<commit_message>
Last commit on 25/10/2023
</commit_message>
<xml_diff>
--- a/Sale Report Excel Comparison/BO_Data_Comparision_Report.xlsx
+++ b/Sale Report Excel Comparison/BO_Data_Comparision_Report.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sappanimuthu.balasub\Documents\LIN_BO_Revamp\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2333C34-CDD0-4860-B9E4-0C796497F9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B2333C34-CDD0-4860-B9E4-0C796497F9A7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{AA5FD2E5-D388-4DEF-A183-91A785FA9E28}"/>
+    <workbookView activeTab="2" windowHeight="10560" windowWidth="19420" xWindow="-110" xr2:uid="{AA5FD2E5-D388-4DEF-A183-91A785FA9E28}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="Both_BO_Value" sheetId="1" r:id="rId1"/>
-    <sheet name="Inside_Values" sheetId="4" r:id="rId2"/>
-    <sheet name="Differences" sheetId="2" r:id="rId3"/>
-    <sheet name="Sales_Report" sheetId="5" r:id="rId4"/>
+    <sheet name="Both_BO_Value" r:id="rId1" sheetId="1"/>
+    <sheet name="Inside_Values" r:id="rId2" sheetId="4"/>
+    <sheet name="Differences" r:id="rId3" sheetId="2"/>
+    <sheet name="Sales_Report" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="204">
   <si>
     <t>Sales</t>
   </si>
@@ -582,13 +582,83 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>19,768.02</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>12.38</t>
+  </si>
+  <si>
+    <t>1,630.64</t>
+  </si>
+  <si>
+    <t>1597</t>
+  </si>
+  <si>
+    <t>1603</t>
+  </si>
+  <si>
+    <t>135.68</t>
+  </si>
+  <si>
+    <t>87.78%</t>
+  </si>
+  <si>
+    <t>21,401.66</t>
+  </si>
+  <si>
+    <t>21,513.66</t>
+  </si>
+  <si>
+    <t>1,182.09</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>3.16</t>
+  </si>
+  <si>
+    <t>2.44%</t>
+  </si>
+  <si>
+    <t>21,592.72</t>
+  </si>
+  <si>
+    <t>0.63%</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2.69%</t>
+  </si>
+  <si>
+    <t>10,859.60</t>
+  </si>
+  <si>
+    <t>2,504.85</t>
+  </si>
+  <si>
+    <t>4,070</t>
+  </si>
+  <si>
+    <t>206.60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="155" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="250" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1215,6 +1285,386 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1261,7 +1711,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="116">
     <border>
       <left/>
       <right/>
@@ -1314,520 +1764,1673 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="267">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="14" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="15" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="16" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="17" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="18" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="19" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="20" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="21" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="24" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="25" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="26" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="28" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="29" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="30" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="31" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="32" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="33" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="34" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="35" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="36" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="37" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="38" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="39" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="40" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="41" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="42" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="43" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="44" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="45" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="46" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="47" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="48" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="49" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="50" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="51" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="52" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="53" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="54" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="55" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="56" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="57" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="58" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="59" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="60" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="61" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="62" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="63" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="64" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="65" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="66" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="67" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="68" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="69" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="70" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="71" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="72" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="73" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="74" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="75" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="76" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="77" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="78" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="115" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="122" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="131" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="134" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="136" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="138" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="140" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="143" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="144" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="145" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="146" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="147" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="148" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="149" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="150" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="151" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="152" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="153" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="154" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="79" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="80" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="81" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="82" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="83" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="84" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="85" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="86" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="87" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="88" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="89" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="90" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="91" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="92" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="93" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="94" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="95" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="96" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="97" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="98" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="99" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="100" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="101" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="102" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="103" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="104" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="105" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="106" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="107" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="108" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="109" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="110" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="111" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="112" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="113" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="114" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="115" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="116" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="117" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="118" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="119" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="120" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="121" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="122" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="123" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="124" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="125" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="126" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="127" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="128" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="129" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="130" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="131" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="132" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="133" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="134" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="135" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="136" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="137" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="138" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="139" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="140" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="141" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="142" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="143" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="144" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="145" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="146" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="147" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="148" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="149" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="150" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="151" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="152" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="153" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="154" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="155" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="156" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="157" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="158" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="159" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="160" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="161" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="162" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="163" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="164" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="165" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="166" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="167" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="168" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="169" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="170" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="171" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="172" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="173" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="174" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="175" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="176" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="177" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="178" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="179" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="180" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="181" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="182" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="11" fillId="0" fontId="183" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="184" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="185" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="186" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="187" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="188" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="189" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="190" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="191" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="192" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="193" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="194" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="195" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="196" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="197" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="198" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="199" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="200" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="201" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="202" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="203" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="204" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="205" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="206" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="207" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="208" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="209" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="210" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="211" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="212" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="19" fillId="0" fontId="213" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="27" fillId="0" fontId="214" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="27" fillId="0" fontId="215" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="27" fillId="0" fontId="216" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="35" fillId="0" fontId="217" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="35" fillId="0" fontId="218" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="35" fillId="0" fontId="219" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="43" fillId="0" fontId="220" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="43" fillId="0" fontId="221" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="43" fillId="0" fontId="222" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="51" fillId="0" fontId="223" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="51" fillId="0" fontId="224" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="51" fillId="0" fontId="225" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="59" fillId="0" fontId="226" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="59" fillId="0" fontId="227" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="59" fillId="0" fontId="228" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="67" fillId="0" fontId="229" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="67" fillId="0" fontId="230" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="67" fillId="0" fontId="231" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="75" fillId="0" fontId="232" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="75" fillId="0" fontId="233" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="75" fillId="0" fontId="234" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="83" fillId="0" fontId="235" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="83" fillId="0" fontId="236" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="83" fillId="0" fontId="237" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="91" fillId="0" fontId="238" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="91" fillId="0" fontId="239" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="91" fillId="0" fontId="240" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="99" fillId="0" fontId="241" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="99" fillId="0" fontId="242" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="99" fillId="0" fontId="243" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="107" fillId="0" fontId="244" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="107" fillId="0" fontId="245" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="107" fillId="0" fontId="246" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="247" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="248" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="249" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="41">
     <dxf>
@@ -2163,7 +3766,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2180,10 +3783,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2218,7 +3821,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2270,7 +3873,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2381,21 +3984,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2412,7 +4015,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2464,14 +4067,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8461D5C9-C633-44D2-A2F6-895739E4A308}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8461D5C9-C633-44D2-A2F6-895739E4A308}">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2480,14 +4083,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.6328125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -3302,7 +4905,9 @@
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="201" t="s">
+        <v>181</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
@@ -3338,7 +4943,9 @@
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="202" t="s">
+        <v>182</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3374,7 +4981,9 @@
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="203" t="s">
+        <v>183</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>180</v>
       </c>
@@ -3410,7 +5019,9 @@
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="204" t="s">
+        <v>183</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>180</v>
       </c>
@@ -3448,7 +5059,9 @@
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="205" t="s">
+        <v>184</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>180</v>
       </c>
@@ -3488,7 +5101,9 @@
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="206" t="s">
+        <v>185</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>180</v>
       </c>
@@ -3534,7 +5149,9 @@
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="207" t="s">
+        <v>186</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>180</v>
       </c>
@@ -3580,7 +5197,9 @@
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="208" t="s">
+        <v>187</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>180</v>
       </c>
@@ -3626,7 +5245,9 @@
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="209" t="s">
+        <v>182</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>180</v>
       </c>
@@ -3672,7 +5293,9 @@
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="210" t="s">
+        <v>199</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>180</v>
       </c>
@@ -3718,7 +5341,9 @@
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="211" t="s">
+        <v>188</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>180</v>
       </c>
@@ -3831,12 +5456,12 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="O20:P20"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AD18B4-AA5C-4DAC-B720-8E364BC00296}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AD18B4-AA5C-4DAC-B720-8E364BC00296}">
   <dimension ref="A1:E396"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
@@ -3845,11 +5470,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4" collapsed="1"/>
-    <col min="2" max="2" width="36" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.36328125" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.36328125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="36.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="12.36328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="11.36328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3875,9 +5500,11 @@
         <v>56</v>
       </c>
       <c r="C2" s="19"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="212" t="s">
+        <v>181</v>
+      </c>
       <c r="E2" s="167">
-        <f t="shared" ref="E2:E45" si="0">C2-D2</f>
+        <f ref="E2:E45" si="0" t="shared">C2-D2</f>
         <v>0</v>
       </c>
     </row>
@@ -3889,7 +5516,9 @@
       <c r="C3" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="213" t="s">
+        <v>184</v>
+      </c>
       <c r="E3" s="167">
         <f>C3-D3</f>
         <v>122.36</v>
@@ -3903,9 +5532,11 @@
       <c r="C4" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="214" t="s">
+        <v>187</v>
+      </c>
       <c r="E4" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -3917,9 +5548,11 @@
       <c r="C5" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="215" t="s">
+        <v>189</v>
+      </c>
       <c r="E5" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -3931,9 +5564,11 @@
       <c r="C6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="216" t="s">
+        <v>184</v>
+      </c>
       <c r="E6" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -3945,9 +5580,11 @@
       <c r="C7" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="217" t="s">
+        <v>102</v>
+      </c>
       <c r="E7" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -3959,9 +5596,11 @@
       <c r="C8" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="218" t="s">
+        <v>102</v>
+      </c>
       <c r="E8" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -3973,9 +5612,11 @@
       <c r="C9" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="219" t="s">
+        <v>102</v>
+      </c>
       <c r="E9" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -3987,9 +5628,11 @@
       <c r="C10" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="220" t="s">
+        <v>190</v>
+      </c>
       <c r="E10" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -4001,9 +5644,11 @@
       <c r="C11" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="221" t="s">
+        <v>191</v>
+      </c>
       <c r="E11" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>87</v>
       </c>
     </row>
@@ -4015,9 +5660,11 @@
       <c r="C12" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="222" t="s">
+        <v>187</v>
+      </c>
       <c r="E12" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -4029,9 +5676,11 @@
       <c r="C13" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="223" t="s">
+        <v>192</v>
+      </c>
       <c r="E13" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
     </row>
@@ -4043,9 +5692,11 @@
       <c r="C14" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="224" t="s">
+        <v>193</v>
+      </c>
       <c r="E14" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>2.4300000000000002</v>
       </c>
     </row>
@@ -4057,9 +5708,11 @@
       <c r="C15" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="225" t="s">
+        <v>185</v>
+      </c>
       <c r="E15" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>124</v>
       </c>
     </row>
@@ -4071,9 +5724,11 @@
       <c r="C16" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="226" t="s">
+        <v>194</v>
+      </c>
       <c r="E16" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>3.2300000000000002E-2</v>
       </c>
     </row>
@@ -4085,9 +5740,11 @@
       <c r="C17" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="227" t="s">
+        <v>195</v>
+      </c>
       <c r="E17" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1616.63</v>
       </c>
     </row>
@@ -4099,9 +5756,11 @@
       <c r="C18" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="228" t="s">
+        <v>196</v>
+      </c>
       <c r="E18" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -4113,9 +5772,11 @@
       <c r="C19" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="229" t="s">
+        <v>197</v>
+      </c>
       <c r="E19" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4</v>
       </c>
     </row>
@@ -4127,7 +5788,7 @@
       <c r="C20" s="37"/>
       <c r="D20" s="6"/>
       <c r="E20" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4139,9 +5800,11 @@
       <c r="C21" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="230" t="s">
+        <v>200</v>
+      </c>
       <c r="E21" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>24.97</v>
       </c>
     </row>
@@ -4153,7 +5816,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4165,7 +5828,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4179,7 +5842,7 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>54.59</v>
       </c>
     </row>
@@ -4193,7 +5856,7 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4.5199999999999996</v>
       </c>
     </row>
@@ -4207,7 +5870,7 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4221,7 +5884,7 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>59.11</v>
       </c>
     </row>
@@ -4235,7 +5898,7 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>54.59</v>
       </c>
     </row>
@@ -4249,7 +5912,7 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4.5199999999999996</v>
       </c>
     </row>
@@ -4263,7 +5926,7 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4277,7 +5940,7 @@
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>59.11</v>
       </c>
     </row>
@@ -4289,7 +5952,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4301,7 +5964,7 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4315,7 +5978,7 @@
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4329,7 +5992,7 @@
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4343,7 +6006,7 @@
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>59.11</v>
       </c>
     </row>
@@ -4357,7 +6020,7 @@
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4369,7 +6032,7 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4381,7 +6044,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4393,7 +6056,7 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4405,7 +6068,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4417,7 +6080,7 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4429,7 +6092,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4441,7 +6104,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -4453,7 +6116,7 @@
       <c r="C45" s="85"/>
       <c r="D45" s="85"/>
       <c r="E45" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -6565,19 +8228,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E45">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule dxfId="28" operator="equal" priority="2" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+    <cfRule dxfId="27" operator="greaterThan" priority="3" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{6A8EA411-9737-410B-803F-B767DF546FBC}">
+          <x14:cfRule id="{6A8EA411-9737-410B-803F-B767DF546FBC}" operator="containsText" priority="1" type="containsText">
             <xm:f>NOT(ISERROR(SEARCH("-",E2)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -6597,7 +8260,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783EEC30-26F5-4E4B-A202-0672BF52BF40}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783EEC30-26F5-4E4B-A202-0672BF52BF40}">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -6606,22 +8269,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.08984375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.54296875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.54296875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.08984375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.54296875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.36328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.6328125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="13.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -7386,88 +9049,88 @@
     <mergeCell ref="O2:P2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B15">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
+    <cfRule dxfId="20" operator="greaterThan" priority="21" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule dxfId="19" operator="equal" priority="20" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
+    <cfRule dxfId="18" operator="lessThan" priority="19" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F8">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="lessThan">
+    <cfRule dxfId="17" operator="lessThan" priority="16" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule dxfId="16" operator="equal" priority="17" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+    <cfRule dxfId="15" operator="greaterThan" priority="18" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H8">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+    <cfRule dxfId="14" operator="lessThan" priority="13" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule dxfId="13" operator="equal" priority="14" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+    <cfRule dxfId="12" operator="greaterThan" priority="15" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
+    <cfRule dxfId="11" operator="lessThan" priority="10" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule dxfId="10" operator="equal" priority="11" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+    <cfRule dxfId="9" operator="greaterThan" priority="12" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L7">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+    <cfRule dxfId="8" operator="lessThan" priority="7" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule dxfId="7" operator="equal" priority="8" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+    <cfRule dxfId="6" operator="greaterThan" priority="9" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N8">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule dxfId="5" operator="lessThan" priority="4" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule dxfId="4" operator="equal" priority="5" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule dxfId="3" operator="greaterThan" priority="6" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule dxfId="2" operator="lessThan" priority="1" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule dxfId="1" operator="equal" priority="2" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule dxfId="0" operator="greaterThan" priority="3" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27932D39-BE19-45BB-BA59-DCA53411D6F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27932D39-BE19-45BB-BA59-DCA53411D6F6}">
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7476,13 +9139,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.6328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" customWidth="1"/>
-    <col min="20" max="20" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="15.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.6328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="19.54296875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="17.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -7528,7 +9191,7 @@
       </c>
       <c r="D3" s="84"/>
       <c r="E3" s="167">
-        <f t="shared" ref="E3:E66" si="0">C3-D3</f>
+        <f ref="E3:E66" si="0" t="shared">C3-D3</f>
         <v>226</v>
       </c>
     </row>
@@ -7542,7 +9205,7 @@
       </c>
       <c r="D4" s="84"/>
       <c r="E4" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -7556,7 +9219,7 @@
       </c>
       <c r="D5" s="84"/>
       <c r="E5" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7570,7 +9233,7 @@
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7586,7 +9249,7 @@
       </c>
       <c r="D7" s="84"/>
       <c r="E7" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -7600,7 +9263,7 @@
       </c>
       <c r="D8" s="84"/>
       <c r="E8" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>226</v>
       </c>
     </row>
@@ -7614,7 +9277,7 @@
       </c>
       <c r="D9" s="84"/>
       <c r="E9" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -7628,7 +9291,7 @@
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7642,7 +9305,7 @@
       </c>
       <c r="D11" s="84"/>
       <c r="E11" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>100</v>
       </c>
     </row>
@@ -7658,7 +9321,7 @@
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1410.04</v>
       </c>
     </row>
@@ -7672,7 +9335,7 @@
       </c>
       <c r="D13" s="84"/>
       <c r="E13" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>214</v>
       </c>
     </row>
@@ -7686,7 +9349,7 @@
       </c>
       <c r="D14" s="84"/>
       <c r="E14" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>116.28</v>
       </c>
     </row>
@@ -7700,7 +9363,7 @@
       </c>
       <c r="D15" s="84"/>
       <c r="E15" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7714,7 +9377,7 @@
       </c>
       <c r="D16" s="84"/>
       <c r="E16" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>100</v>
       </c>
     </row>
@@ -7730,7 +9393,7 @@
       </c>
       <c r="D17" s="84"/>
       <c r="E17" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -7744,7 +9407,7 @@
       </c>
       <c r="D18" s="84"/>
       <c r="E18" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>226</v>
       </c>
     </row>
@@ -7758,7 +9421,7 @@
       </c>
       <c r="D19" s="84"/>
       <c r="E19" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -7772,7 +9435,7 @@
       </c>
       <c r="D20" s="84"/>
       <c r="E20" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7786,7 +9449,7 @@
       </c>
       <c r="D21" s="84"/>
       <c r="E21" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>100</v>
       </c>
     </row>
@@ -7800,9 +9463,11 @@
       <c r="C22" s="106" t="s">
         <v>177</v>
       </c>
-      <c r="D22" s="84"/>
+      <c r="D22" s="264" t="s">
+        <v>201</v>
+      </c>
       <c r="E22" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>179.55</v>
       </c>
     </row>
@@ -7814,9 +9479,11 @@
       <c r="C23" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="D23" s="84"/>
+      <c r="D23" s="265" t="s">
+        <v>202</v>
+      </c>
       <c r="E23" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>295</v>
       </c>
     </row>
@@ -7828,9 +9495,11 @@
       <c r="C24" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="D24" s="84"/>
+      <c r="D24" s="266" t="s">
+        <v>203</v>
+      </c>
       <c r="E24" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>14.81</v>
       </c>
     </row>
@@ -7846,7 +9515,7 @@
       </c>
       <c r="D25" s="84"/>
       <c r="E25" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -7860,7 +9529,7 @@
       </c>
       <c r="D26" s="84"/>
       <c r="E26" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -7874,7 +9543,7 @@
       </c>
       <c r="D27" s="84"/>
       <c r="E27" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>226</v>
       </c>
     </row>
@@ -7888,7 +9557,7 @@
       </c>
       <c r="D28" s="84"/>
       <c r="E28" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7902,7 +9571,7 @@
       </c>
       <c r="D29" s="84"/>
       <c r="E29" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -7916,7 +9585,7 @@
       </c>
       <c r="D30" s="84"/>
       <c r="E30" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>124</v>
       </c>
     </row>
@@ -7932,7 +9601,7 @@
       </c>
       <c r="D31" s="84"/>
       <c r="E31" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -7946,7 +9615,7 @@
       </c>
       <c r="D32" s="84"/>
       <c r="E32" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -7960,7 +9629,7 @@
       </c>
       <c r="D33" s="84"/>
       <c r="E33" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -7974,7 +9643,7 @@
       </c>
       <c r="D34" s="84"/>
       <c r="E34" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -7990,7 +9659,7 @@
       </c>
       <c r="D35" s="84"/>
       <c r="E35" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -8004,7 +9673,7 @@
       </c>
       <c r="D36" s="84"/>
       <c r="E36" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -8018,7 +9687,7 @@
       </c>
       <c r="D37" s="84"/>
       <c r="E37" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -8032,7 +9701,7 @@
       </c>
       <c r="D38" s="84"/>
       <c r="E38" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -8046,7 +9715,7 @@
       </c>
       <c r="D39" s="84"/>
       <c r="E39" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -8060,7 +9729,7 @@
       </c>
       <c r="D40" s="84"/>
       <c r="E40" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1616.63</v>
       </c>
     </row>
@@ -8074,7 +9743,7 @@
       </c>
       <c r="D41" s="84"/>
       <c r="E41" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8088,7 +9757,7 @@
       </c>
       <c r="D42" s="84"/>
       <c r="E42" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8102,7 +9771,7 @@
       </c>
       <c r="D43" s="84"/>
       <c r="E43" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8114,7 +9783,7 @@
       <c r="C44" s="84"/>
       <c r="D44" s="84"/>
       <c r="E44" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8128,7 +9797,7 @@
       </c>
       <c r="D45" s="84"/>
       <c r="E45" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>-6.9099999999999995E-2</v>
       </c>
     </row>
@@ -8142,7 +9811,7 @@
       </c>
       <c r="D46" s="84"/>
       <c r="E46" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8158,7 +9827,7 @@
       </c>
       <c r="D47" s="84"/>
       <c r="E47" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -8172,7 +9841,7 @@
       </c>
       <c r="D48" s="84"/>
       <c r="E48" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -8186,7 +9855,7 @@
       </c>
       <c r="D49" s="84"/>
       <c r="E49" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -8200,7 +9869,7 @@
       </c>
       <c r="D50" s="84"/>
       <c r="E50" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -8214,7 +9883,7 @@
       </c>
       <c r="D51" s="84"/>
       <c r="E51" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -8228,7 +9897,7 @@
       </c>
       <c r="D52" s="84"/>
       <c r="E52" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1616.63</v>
       </c>
     </row>
@@ -8242,7 +9911,7 @@
       </c>
       <c r="D53" s="84"/>
       <c r="E53" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8256,7 +9925,7 @@
       </c>
       <c r="D54" s="84"/>
       <c r="E54" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8270,7 +9939,7 @@
       </c>
       <c r="D55" s="84"/>
       <c r="E55" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8282,7 +9951,7 @@
       <c r="C56" s="84"/>
       <c r="D56" s="84"/>
       <c r="E56" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8296,7 +9965,7 @@
       </c>
       <c r="D57" s="84"/>
       <c r="E57" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>-6.9099999999999995E-2</v>
       </c>
     </row>
@@ -8310,7 +9979,7 @@
       </c>
       <c r="D58" s="84"/>
       <c r="E58" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8326,7 +9995,7 @@
       </c>
       <c r="D59" s="84"/>
       <c r="E59" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>13169.84</v>
       </c>
     </row>
@@ -8340,7 +10009,7 @@
       </c>
       <c r="D60" s="84"/>
       <c r="E60" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>14380.02</v>
       </c>
     </row>
@@ -8354,7 +10023,7 @@
       </c>
       <c r="D61" s="84"/>
       <c r="E61" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>14257.09</v>
       </c>
     </row>
@@ -8368,7 +10037,7 @@
       </c>
       <c r="D62" s="84"/>
       <c r="E62" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>11.83</v>
       </c>
     </row>
@@ -8382,7 +10051,7 @@
       </c>
       <c r="D63" s="84"/>
       <c r="E63" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>12.8</v>
       </c>
     </row>
@@ -8396,7 +10065,7 @@
       </c>
       <c r="D64" s="84"/>
       <c r="E64" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>14345.09</v>
       </c>
     </row>
@@ -8410,7 +10079,7 @@
       </c>
       <c r="D65" s="84"/>
       <c r="E65" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1086.25</v>
       </c>
     </row>
@@ -8424,7 +10093,7 @@
       </c>
       <c r="D66" s="84"/>
       <c r="E66" s="167">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8438,7 +10107,7 @@
       </c>
       <c r="D67" s="84"/>
       <c r="E67" s="167">
-        <f t="shared" ref="E67:E79" si="1">C67-D67</f>
+        <f ref="E67:E79" si="1" t="shared">C67-D67</f>
         <v>0</v>
       </c>
     </row>
@@ -8454,7 +10123,7 @@
       </c>
       <c r="D68" s="84"/>
       <c r="E68" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>1483.76</v>
       </c>
     </row>
@@ -8468,7 +10137,7 @@
       </c>
       <c r="D69" s="84"/>
       <c r="E69" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>122.36</v>
       </c>
     </row>
@@ -8482,7 +10151,7 @@
       </c>
       <c r="D70" s="84"/>
       <c r="E70" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8496,7 +10165,7 @@
       </c>
       <c r="D71" s="84"/>
       <c r="E71" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8510,7 +10179,7 @@
       </c>
       <c r="D72" s="84"/>
       <c r="E72" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>9.7100000000000009</v>
       </c>
     </row>
@@ -8524,7 +10193,7 @@
       </c>
       <c r="D73" s="84"/>
       <c r="E73" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>1606.12</v>
       </c>
     </row>
@@ -8540,7 +10209,7 @@
       </c>
       <c r="D74" s="84"/>
       <c r="E74" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>9.8000000000000007</v>
       </c>
     </row>
@@ -8554,7 +10223,7 @@
       </c>
       <c r="D75" s="84"/>
       <c r="E75" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8568,7 +10237,7 @@
       </c>
       <c r="D76" s="84"/>
       <c r="E76" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0.81</v>
       </c>
     </row>
@@ -8582,7 +10251,7 @@
       </c>
       <c r="D77" s="84"/>
       <c r="E77" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8596,7 +10265,7 @@
       </c>
       <c r="D78" s="84"/>
       <c r="E78" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>0</v>
       </c>
     </row>
@@ -8610,7 +10279,7 @@
       </c>
       <c r="D79" s="84"/>
       <c r="E79" s="167">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>10.61</v>
       </c>
     </row>
@@ -8630,20 +10299,20 @@
     <mergeCell ref="A7:A11"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:E79">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
+    <cfRule dxfId="26" operator="greaterThan" priority="2" type="cellIs">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule dxfId="25" operator="equal" priority="3" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{D7146347-276E-45E1-99C3-0065D877768D}">
+          <x14:cfRule id="{D7146347-276E-45E1-99C3-0065D877768D}" operator="containsText" priority="1" type="containsText">
             <xm:f>NOT(ISERROR(SEARCH("-",E1)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
Last Update on 26/10/2023
</commit_message>
<xml_diff>
--- a/Sale Report Excel Comparison/BO_Data_Comparision_Report.xlsx
+++ b/Sale Report Excel Comparison/BO_Data_Comparision_Report.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="213">
   <si>
     <t>Sales</t>
   </si>
@@ -651,6 +651,33 @@
   </si>
   <si>
     <t>206.60</t>
+  </si>
+  <si>
+    <t>1,026.03</t>
+  </si>
+  <si>
+    <t>1,110.79</t>
+  </si>
+  <si>
+    <t>84.76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>41.36</t>
+  </si>
+  <si>
+    <t>3.4300</t>
+  </si>
+  <si>
+    <t>46.79</t>
+  </si>
+  <si>
+    <t>84.39</t>
+  </si>
+  <si>
+    <t>3.00</t>
   </si>
 </sst>
 </file>
@@ -658,7 +685,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="250" x14ac:knownFonts="1">
+  <fonts count="269" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,6 +1312,82 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1711,7 +1814,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="116">
+  <borders count="124">
     <border>
       <left/>
       <right/>
@@ -2632,11 +2735,73 @@
         <color indexed="8"/>
       </bottom>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="286">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
@@ -3419,13 +3584,70 @@
     <xf applyBorder="true" applyFont="true" borderId="107" fillId="0" fontId="246" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="247" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="248" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="249" fillId="0" borderId="115" xfId="0" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFont="true" borderId="115" fillId="0" fontId="247" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="115" fillId="0" fontId="248" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="115" fillId="0" fontId="249" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="250" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="251" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="252" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="253" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="254" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="255" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="256" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="257" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="258" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="259" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="260" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="261" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="262" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="263" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="264" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="265" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="266" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="267" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="268" fillId="0" borderId="123" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4933,7 +5155,9 @@
       <c r="M22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="267" t="s">
+        <v>204</v>
+      </c>
       <c r="O22" s="1" t="s">
         <v>39</v>
       </c>
@@ -4971,7 +5195,9 @@
       <c r="M23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="268" t="s">
+        <v>205</v>
+      </c>
       <c r="O23" s="1" t="s">
         <v>40</v>
       </c>
@@ -5009,7 +5235,9 @@
       <c r="M24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="269" t="s">
+        <v>206</v>
+      </c>
       <c r="O24" s="1" t="s">
         <v>41</v>
       </c>
@@ -5049,7 +5277,9 @@
       <c r="M25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="270" t="s">
+        <v>207</v>
+      </c>
       <c r="O25" s="1" t="s">
         <v>42</v>
       </c>
@@ -5091,7 +5321,9 @@
       <c r="M26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="1"/>
+      <c r="N26" s="271" t="s">
+        <v>102</v>
+      </c>
       <c r="O26" s="1" t="s">
         <v>43</v>
       </c>
@@ -5840,7 +6072,9 @@
       <c r="C24" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="272" t="s">
+        <v>208</v>
+      </c>
       <c r="E24" s="167">
         <f si="0" t="shared"/>
         <v>54.59</v>
@@ -5854,7 +6088,9 @@
       <c r="C25" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="273" t="s">
+        <v>209</v>
+      </c>
       <c r="E25" s="167">
         <f si="0" t="shared"/>
         <v>4.5199999999999996</v>
@@ -5868,7 +6104,9 @@
       <c r="C26" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="274" t="s">
+        <v>102</v>
+      </c>
       <c r="E26" s="167">
         <f si="0" t="shared"/>
         <v>0</v>
@@ -5882,7 +6120,9 @@
       <c r="C27" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="275" t="s">
+        <v>210</v>
+      </c>
       <c r="E27" s="167">
         <f si="0" t="shared"/>
         <v>59.11</v>
@@ -5896,7 +6136,9 @@
       <c r="C28" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="276" t="s">
+        <v>208</v>
+      </c>
       <c r="E28" s="167">
         <f si="0" t="shared"/>
         <v>54.59</v>
@@ -5910,7 +6152,9 @@
       <c r="C29" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="277" t="s">
+        <v>209</v>
+      </c>
       <c r="E29" s="167">
         <f si="0" t="shared"/>
         <v>4.5199999999999996</v>
@@ -5924,7 +6168,9 @@
       <c r="C30" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="278" t="s">
+        <v>102</v>
+      </c>
       <c r="E30" s="167">
         <f si="0" t="shared"/>
         <v>0</v>
@@ -5938,7 +6184,9 @@
       <c r="C31" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="6"/>
+      <c r="D31" s="279" t="s">
+        <v>210</v>
+      </c>
       <c r="E31" s="167">
         <f si="0" t="shared"/>
         <v>59.11</v>
@@ -5950,7 +6198,9 @@
         <v>87</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+      <c r="D32" s="280" t="s">
+        <v>211</v>
+      </c>
       <c r="E32" s="167">
         <f si="0" t="shared"/>
         <v>0</v>
@@ -5962,7 +6212,9 @@
         <v>88</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="281" t="s">
+        <v>102</v>
+      </c>
       <c r="E33" s="167">
         <f si="0" t="shared"/>
         <v>0</v>
@@ -5976,7 +6228,9 @@
       <c r="C34" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="282" t="s">
+        <v>102</v>
+      </c>
       <c r="E34" s="167">
         <f si="0" t="shared"/>
         <v>0</v>
@@ -5990,7 +6244,9 @@
       <c r="C35" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="283" t="s">
+        <v>102</v>
+      </c>
       <c r="E35" s="167">
         <f si="0" t="shared"/>
         <v>0</v>
@@ -6004,7 +6260,9 @@
       <c r="C36" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="6"/>
+      <c r="D36" s="284" t="s">
+        <v>205</v>
+      </c>
       <c r="E36" s="167">
         <f si="0" t="shared"/>
         <v>59.11</v>
@@ -6018,7 +6276,9 @@
       <c r="C37" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="6"/>
+      <c r="D37" s="285" t="s">
+        <v>212</v>
+      </c>
       <c r="E37" s="167">
         <f si="0" t="shared"/>
         <v>0</v>

</xml_diff>

<commit_message>
Healenium added to all the suites & Updated on 06/11/2023
</commit_message>
<xml_diff>
--- a/Sale Report Excel Comparison/BO_Data_Comparision_Report.xlsx
+++ b/Sale Report Excel Comparison/BO_Data_Comparision_Report.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="234">
   <si>
     <t>Sales</t>
   </si>
@@ -735,6 +735,12 @@
   </si>
   <si>
     <t>3.00</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>00:00</t>
   </si>
 </sst>
 </file>
@@ -742,7 +748,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="234" x14ac:knownFonts="1">
+  <fonts count="240" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1822,6 +1828,30 @@
       <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1944,7 +1974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -2104,11 +2134,135 @@
         <color indexed="8"/>
       </bottom>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="250">
+  <cellXfs count="256">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
@@ -2792,61 +2946,79 @@
     <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="215" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="216" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="217" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="218" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="219" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="220" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="221" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="222" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="223" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="224" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="225" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="226" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="227" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="228" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="229" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="230" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="231" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="232" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="233" fillId="0" borderId="14" xfId="0" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="215" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="216" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="217" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="218" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="219" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="220" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="221" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="222" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="223" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="224" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="225" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="226" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="227" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="228" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="229" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="230" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="231" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="232" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="14" fillId="0" fontId="233" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="22" fillId="0" fontId="234" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="22" fillId="0" fontId="235" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="true" applyFont="true" borderId="22" fillId="0" fontId="236" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="237" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="238" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="239" fillId="0" borderId="30" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4244,7 +4416,9 @@
       <c r="O22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P22" s="1"/>
+      <c r="P22" s="250" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -4262,7 +4436,9 @@
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="253" t="s">
+        <v>120</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>28</v>
       </c>
@@ -4302,7 +4478,9 @@
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="254" t="s">
+        <v>209</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>29</v>
       </c>
@@ -4384,7 +4562,9 @@
       <c r="E26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="255" t="s">
+        <v>233</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>224</v>
       </c>
@@ -4602,7 +4782,9 @@
       <c r="O30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P30" s="1"/>
+      <c r="P30" s="251" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -4650,7 +4832,9 @@
       <c r="O31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P31" s="1"/>
+      <c r="P31" s="252" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">

</xml_diff>